<commit_message>
[task] Update timings 	- Fix timings using newest code 	- Add Rate Monotonic Calculations to Excel file
</commit_message>
<xml_diff>
--- a/Documentation/Execution Durations.xlsx
+++ b/Documentation/Execution Durations.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD1B0AA-9E63-4171-B53B-BAA0255A3C50}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D317719-2760-4805-894B-8D5500FEA3F5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11775" yWindow="4125" windowWidth="21600" windowHeight="11385" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4215" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
   <si>
     <t>CONFIG_MODE</t>
   </si>
@@ -433,11 +433,11 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>4361700</v>
+        <v>2694699</v>
       </c>
       <c r="B2">
         <f>AVERAGE(A2)</f>
-        <v>4361700</v>
+        <v>2694699</v>
       </c>
     </row>
   </sheetData>
@@ -447,7 +447,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27CF55B4-E905-40BA-9696-012140E111F6}">
-  <dimension ref="A1:B185"/>
+  <dimension ref="A1:B193"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -469,926 +469,966 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>166800</v>
+        <v>550800</v>
       </c>
       <c r="B2">
-        <f>AVERAGE(A2:A185)</f>
-        <v>1156930709.2391305</v>
+        <f>AVERAGE(A2:A193)</f>
+        <v>1615893401.5625</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>5006050200</v>
+        <v>2002028399</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>234400</v>
+        <v>1014223900</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>216500</v>
+        <v>964300</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4000879500</v>
+        <v>16383700</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1003577800</v>
+        <v>1985456300</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>121100</v>
+        <v>2005139900</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>85100</v>
+        <v>1003481301</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>3025496500</v>
+        <v>3035796999</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1005604900</v>
+        <v>1000933200</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>969426400</v>
+        <v>1059701</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2025294900</v>
+        <v>2003170699</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>1008652700</v>
+        <v>29705600</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>968086800</v>
+        <v>1002596800</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>3601200</v>
+        <v>964809400</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>25500</v>
+        <v>1043006500</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>1018590200</v>
+        <v>1004641501</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>1011166500</v>
+        <v>970679500</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>970065400</v>
+        <v>45654000</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>1998563800</v>
+        <v>1004889200</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>30229600</v>
+        <v>974525300</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>1013626600</v>
+        <v>2046937100</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>968090800</v>
+        <v>437700</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>1997309600</v>
+        <v>54085701</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>1015468400</v>
+        <v>976883200</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>49633300</v>
+        <v>966262900</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>970782100</v>
+        <v>51651201</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>17740100</v>
+        <v>1949111200</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>19200</v>
+        <v>38824700</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>4800</v>
+        <v>1066012599</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>8000</v>
+        <v>1947640901</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>193500</v>
+        <v>37589300</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>450900</v>
+        <v>72406699</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>1989623400</v>
+        <v>1946132600</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>1011318400</v>
+        <v>38438099</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>1995298100</v>
+        <v>1962404700</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>1027737100</v>
+        <v>1053431800</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>1008987500</v>
+        <v>1061047000</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>2002440100</v>
+        <v>1963365600</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>33190200</v>
+        <v>1055095900</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>1006513300</v>
+        <v>65146400</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>2000013100</v>
+        <v>1963941400</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>1990213100</v>
+        <v>1054457901</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>47740300</v>
+        <v>944880200</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>2000452000</v>
+        <v>1030624699</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>1990644400</v>
+        <v>20693899</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>1009397900</v>
+        <v>3044733301</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>1049978300</v>
+        <v>1031316000</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>35500</v>
+        <v>20586599</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>184500</v>
+        <v>101582399</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>11600</v>
+        <v>1943922300</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>25000</v>
+        <v>1049820699</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>27200</v>
+        <v>2005457200</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>56015400</v>
+        <v>1054252300</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>1991612800</v>
+        <v>56445900</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>35000</v>
+        <v>992004700</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>87500</v>
+        <v>53546400</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>1998628000</v>
+        <v>54709300</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>1051381600</v>
+        <v>1944225700</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>7600</v>
+        <v>55900400</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>59900</v>
+        <v>1062357700</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>24600</v>
+        <v>54147499</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>19900</v>
+        <v>1946865100</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>338300</v>
+        <v>53783000</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>423100</v>
+        <v>2073882300</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>312900</v>
+        <v>52947501</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>43800</v>
+        <v>1947027200</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>73594400</v>
+        <v>54668800</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>49400</v>
+        <v>3077553100</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>1974063800</v>
+        <v>52891800</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>523361700</v>
+        <v>25500</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>18500</v>
+        <v>2080305901</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>47700</v>
+        <v>55252700</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>35100</v>
+        <v>2865531899</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>549700</v>
+        <v>2078480501</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>518894500</v>
+        <v>53080701</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>498657400</v>
+        <v>1947722601</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>44100</v>
+        <v>51081700</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>3048493000</v>
+        <v>861044801</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>528342400</v>
+        <v>4088946100</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>496240400</v>
+        <v>49433100</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>2050910400</v>
+        <v>858707700</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>532512900</v>
+        <v>1088651800</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>40100</v>
+        <v>3048776200</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>200100</v>
+        <v>862347099</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>1049809300</v>
+        <v>1087695300</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>534407600</v>
+        <v>912809500</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>499980600</v>
+        <v>2132891700</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>349100</v>
+        <v>1951664999</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>207800</v>
+        <v>913502600</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>99900</v>
+        <v>2131937100</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>348900</v>
+        <v>1954332399</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>492604200</v>
+        <v>913124000</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>3960646000</v>
+        <v>2130002001</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>544892800</v>
+        <v>1953476400</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>33600</v>
+        <v>913508200</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>37400</v>
+        <v>2131660400</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>3952020000</v>
+        <v>1950682401</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>547099600</v>
+        <v>49760900</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>498012400</v>
+        <v>864496300</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>3949175500</v>
+        <v>4084089400</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>551036100</v>
+        <v>48678400</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>497125000</v>
+        <v>866185700</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>3944820600</v>
+        <v>4083503400</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>557109600</v>
+        <v>49104201</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>35600</v>
+        <v>864318900</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>185000</v>
+        <v>1081286300</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>303700</v>
+        <v>3053949000</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>530000</v>
+        <v>862735500</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>552948200</v>
+        <v>1082279900</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>501742800</v>
+        <v>3053713200</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>3935172200</v>
+        <v>863272400</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>560704800</v>
+        <v>1081922600</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>6400</v>
+        <v>2002332601</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>9500</v>
+        <v>1049768700</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>3933981800</v>
+        <v>865651899</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>560906800</v>
+        <v>3083420100</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>505368100</v>
+        <v>1046967700</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>3932494900</v>
+        <v>865712500</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>562466500</v>
+        <v>3083352000</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122">
-        <v>505186900</v>
+        <v>1047339799</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>8900</v>
+        <v>866973700</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>5500</v>
+        <v>1132986400</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>562655000</v>
+        <v>1947794700</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>505317600</v>
+        <v>1917560400</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>3929891300</v>
+        <v>1132184299</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>565413300</v>
+        <v>1946683800</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>504097900</v>
+        <v>1921808900</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>3929283500</v>
+        <v>1131585401</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>566826200</v>
+        <v>1944733600</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>36500</v>
+        <v>3055736400</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>31300</v>
+        <v>1943499601</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>3923184400</v>
+        <v>3056187800</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>566682600</v>
+        <v>1944336700</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>509214800</v>
+        <v>3054364600</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>126100</v>
+        <v>1946663199</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138">
-        <v>134400</v>
+        <v>3053458500</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>568293600</v>
+        <v>1946301399</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>508422400</v>
+        <v>3053573499</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>78200</v>
+        <v>1946186600</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>351300</v>
+        <v>3053063200</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143">
-        <v>568697800</v>
+        <v>1946561300</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144">
-        <v>20900</v>
+        <v>52792200</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>18000</v>
+        <v>4946307400</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146">
-        <v>190800</v>
+        <v>54071799</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147">
-        <v>193900</v>
+        <v>4944059100</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148">
-        <v>570446600</v>
+        <v>56365800</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149">
-        <v>4423536400</v>
+        <v>4941023101</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>574635700</v>
+        <v>60587700</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151">
-        <v>39900</v>
+        <v>4939408900</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152">
-        <v>40200</v>
+        <v>59240700</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153">
-        <v>573017400</v>
+        <v>4940477800</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154">
-        <v>4420961400</v>
+        <v>60832500</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155">
-        <v>579591000</v>
+        <v>4940691399</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156">
-        <v>4417855400</v>
+        <v>59852700</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157">
-        <v>582504600</v>
+        <v>4937964300</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158">
-        <v>102500</v>
+        <v>64054300</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159">
-        <v>34900</v>
+        <v>4935822200</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160">
-        <v>25000</v>
+        <v>62584499</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161">
-        <v>40100</v>
+        <v>1939017500</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162">
-        <v>45300</v>
+        <v>3060801300</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163">
-        <v>29300</v>
+        <v>1938913300</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164">
-        <v>589227600</v>
+        <v>1999716899</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165">
-        <v>19800</v>
+        <v>1060145600</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166">
-        <v>597538300</v>
+        <v>3942160399</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167">
-        <v>5500</v>
+        <v>1056568200</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168">
-        <v>602536700</v>
+        <v>3943298601</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169">
-        <v>5001482000</v>
+        <v>1057295500</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170">
-        <v>5001591800</v>
+        <v>3942332099</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171">
-        <v>5000317700</v>
+        <v>1058637601</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172">
-        <v>5001198400</v>
+        <v>3940817201</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173">
-        <v>5001353300</v>
+        <v>1057439200</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174">
-        <v>5000563200</v>
+        <v>3942960500</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175">
-        <v>5000893500</v>
+        <v>1056415200</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176">
-        <v>5001702700</v>
+        <v>3943896500</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177">
-        <v>5000923800</v>
+        <v>1056419300</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178">
-        <v>5000363800</v>
+        <v>3941222400</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179">
-        <v>5000637700</v>
+        <v>1058994200</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180">
-        <v>4999762600</v>
+        <v>3942057400</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181">
-        <v>5000320000</v>
+        <v>6400</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182">
-        <v>5000161600</v>
+        <v>945147800</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183">
-        <v>5002345400</v>
+        <v>4053740100</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184">
-        <v>10700</v>
+        <v>946007101</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185">
-        <v>13200</v>
+        <v>4052466401</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>947570799</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>2002085900</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>5002328600</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>5001104701</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>5000554501</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>6601</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>5000678200</v>
       </c>
     </row>
   </sheetData>
@@ -1398,7 +1438,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A552B6D-2427-4C5B-9654-EE291F958A9A}">
-  <dimension ref="A1:B184"/>
+  <dimension ref="A1:B193"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -1420,921 +1460,966 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>102600</v>
+        <v>1795300</v>
       </c>
       <c r="B2">
-        <f>AVERAGE(A2:A184)</f>
-        <v>355579485.79234976</v>
+        <f>AVERAGE(A2:A193)</f>
+        <v>42206079.203125</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1256500</v>
+        <v>243800</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3585700</v>
+        <v>1125200</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>992600</v>
+        <v>1432000</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>213000</v>
+        <v>757699</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>545000</v>
+        <v>1253200</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>396000</v>
+        <v>982101</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>291500</v>
+        <v>606800</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>133200</v>
+        <v>348601</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>228900</v>
+        <v>404801</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>678800</v>
+        <v>1439300</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>107500</v>
+        <v>726000</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>985300</v>
+        <v>573100</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>1033900</v>
+        <v>1184599</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2473000</v>
+        <v>277499</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>58600</v>
+        <v>240299</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>397700</v>
+        <v>33400</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>253200</v>
+        <v>46100</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>197200</v>
+        <v>108399</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>453300</v>
+        <v>19101</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>121300</v>
+        <v>445300</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>482100</v>
+        <v>208901</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>844600</v>
+        <v>58200</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>18500</v>
+        <v>148000</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>13700</v>
+        <v>406900</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>146700</v>
+        <v>78599</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>534700</v>
+        <v>381400</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>152800</v>
+        <v>872000</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>1013392900</v>
+        <v>29701</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>15600</v>
+        <v>490000</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>1016539800</v>
+        <v>239099</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>28424800</v>
+        <v>74500</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>266300</v>
+        <v>60800</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>71000</v>
+        <v>162201</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>67100</v>
+        <v>26299</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>440300</v>
+        <v>368300</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>220400</v>
+        <v>388401</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>53300</v>
+        <v>43000</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>481700</v>
+        <v>212500</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>386100</v>
+        <v>50500</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>574200</v>
+        <v>437400</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>13500</v>
+        <v>49300</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>88400</v>
+        <v>61400</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>62900</v>
+        <v>55300</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>42900</v>
+        <v>465700</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>14100</v>
+        <v>66501</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>17700</v>
+        <v>70199</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>58800</v>
+        <v>232900</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>1988973800</v>
+        <v>282000</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>327200</v>
+        <v>16400</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>1003261600</v>
+        <v>36799</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>20800</v>
+        <v>68300</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>233300</v>
+        <v>381700</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>404500</v>
+        <v>286400</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>115100</v>
+        <v>24299</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>1006137500</v>
+        <v>594799</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>471700</v>
+        <v>422101</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>105400</v>
+        <v>56301</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>706100</v>
+        <v>45800</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>1006767000</v>
+        <v>461000</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>45900</v>
+        <v>83201</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>2003233600</v>
+        <v>21300</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>33900</v>
+        <v>255000</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>56250700</v>
+        <v>302900</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>218700</v>
+        <v>392600</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>1007145900</v>
+        <v>97400</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>81200</v>
+        <v>28500</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>1486000</v>
+        <v>414701</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>260500</v>
+        <v>375601</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>357700</v>
+        <v>429400</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>72351000</v>
+        <v>37700</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>38200</v>
+        <v>78100</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>3977591800</v>
+        <v>53700</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>319600</v>
+        <v>85300</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>42500</v>
+        <v>57401</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>388300</v>
+        <v>412700</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>60900</v>
+        <v>66300</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>101100</v>
+        <v>26700</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>54200</v>
+        <v>47201</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>18900</v>
+        <v>273500</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>468900</v>
+        <v>47900</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>389600</v>
+        <v>305800</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>495303200</v>
+        <v>57400</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>197300</v>
+        <v>186799</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>327600</v>
+        <v>325599</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>25300</v>
+        <v>386200</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>81400</v>
+        <v>322201</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>52781500</v>
+        <v>308299</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>187500</v>
+        <v>295199</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>535580000</v>
+        <v>79599</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>238700</v>
+        <v>20500</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>34400</v>
+        <v>207200</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>56400</v>
+        <v>97299</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>23200</v>
+        <v>89600</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>496675800</v>
+        <v>505500</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>76400</v>
+        <v>83801</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>747900</v>
+        <v>433300</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>392300</v>
+        <v>13999</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>277700</v>
+        <v>286700</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>423500</v>
+        <v>188100</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>308300</v>
+        <v>361200</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>315000</v>
+        <v>24700</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>116000</v>
+        <v>219500</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>88800</v>
+        <v>537300</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>497812900</v>
+        <v>660500</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>80400</v>
+        <v>269599</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>3940274700</v>
+        <v>12600</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>432200</v>
+        <v>81799</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>258300</v>
+        <v>38200</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>229000</v>
+        <v>115501</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>88200</v>
+        <v>146001</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>26300</v>
+        <v>17200</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>504304900</v>
+        <v>45500</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>15900</v>
+        <v>85001</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>63200</v>
+        <v>17600</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>17800</v>
+        <v>58100</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>392700</v>
+        <v>1379000</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>26100</v>
+        <v>271901</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>17100</v>
+        <v>395400</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>18400</v>
+        <v>228400</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122">
-        <v>3931745700</v>
+        <v>381100</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>110100</v>
+        <v>220500</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>19900</v>
+        <v>58301</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>17700</v>
+        <v>43801</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>30100</v>
+        <v>244000</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>96000</v>
+        <v>89400</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>22800</v>
+        <v>29699</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>135400</v>
+        <v>225701</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>400700</v>
+        <v>92800</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>503894600</v>
+        <v>44700</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>226600</v>
+        <v>65900</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>395800</v>
+        <v>87400</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>93600</v>
+        <v>81800</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>241900</v>
+        <v>308300</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>3919715300</v>
+        <v>27900</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>52600</v>
+        <v>44199</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138">
-        <v>54500</v>
+        <v>58401</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>231600</v>
+        <v>58800</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>3918086400</v>
+        <v>42501</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>202900</v>
+        <v>341300</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>43900</v>
+        <v>42700</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143">
-        <v>509311500</v>
+        <v>244000</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144">
-        <v>408200</v>
+        <v>195800</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>3912785200</v>
+        <v>69400</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146">
-        <v>86100</v>
+        <v>65999</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147">
-        <v>33300</v>
+        <v>272600</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148">
-        <v>205600</v>
+        <v>207900</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149">
-        <v>139700</v>
+        <v>16600</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>4424174100</v>
+        <v>418400</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151">
-        <v>81100</v>
+        <v>230900</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152">
-        <v>57800</v>
+        <v>23101</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153">
-        <v>55100</v>
+        <v>17900</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154">
-        <v>116900</v>
+        <v>33999</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155">
-        <v>66600</v>
+        <v>46900</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156">
-        <v>355800</v>
+        <v>104200</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157">
-        <v>4415900500</v>
+        <v>25899</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158">
-        <v>79500</v>
+        <v>197700</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159">
-        <v>581805700</v>
+        <v>210800</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160">
-        <v>51800</v>
+        <v>63500</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161">
-        <v>4408136700</v>
+        <v>251000</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162">
-        <v>1300600</v>
+        <v>228100</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163">
-        <v>83400</v>
+        <v>44199</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164">
-        <v>4403192200</v>
+        <v>17000</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165">
-        <v>53900</v>
+        <v>23500</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166">
-        <v>4399578100</v>
+        <v>329400</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167">
-        <v>43600</v>
+        <v>154801</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168">
-        <v>71200</v>
+        <v>25301</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169">
-        <v>42400</v>
+        <v>158901</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170">
-        <v>10700</v>
+        <v>151500</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171">
-        <v>72300</v>
+        <v>84101</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172">
-        <v>50100</v>
+        <v>618601</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173">
-        <v>21300</v>
+        <v>31100</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174">
-        <v>11800</v>
+        <v>382900</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175">
-        <v>39200</v>
+        <v>227700</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176">
-        <v>9100</v>
+        <v>192601</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177">
-        <v>20700</v>
+        <v>146500</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178">
-        <v>60400</v>
+        <v>13001</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179">
-        <v>19000</v>
+        <v>23300</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180">
-        <v>14500</v>
+        <v>315800</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181">
-        <v>110300</v>
+        <v>1057183699</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182">
-        <v>626200</v>
+        <v>686300</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183">
-        <v>5000847600</v>
+        <v>85401</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184">
-        <v>388900</v>
+        <v>395901</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>47600</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>17100</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>81800</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>45300</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>55099</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>2001066100</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>147300</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>5000012799</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>87000</v>
       </c>
     </row>
   </sheetData>
@@ -2376,7 +2461,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0CCD4D2-9565-453E-B39F-A0279516BB5B}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -2398,76 +2483,106 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>457500</v>
+        <v>4825199</v>
       </c>
       <c r="B2">
-        <f>AVERAGE(A2:A15)</f>
-        <v>409642.85714285716</v>
+        <f>AVERAGE(A2:A21)</f>
+        <v>1471479.8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>308100</v>
+        <v>1946500</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>381200</v>
+        <v>4044199</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>214500</v>
+        <v>923101</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>326600</v>
+        <v>3413600</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>145800</v>
+        <v>813399</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>223000</v>
+        <v>1030600</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>602300</v>
+        <v>3023400</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>885100</v>
+        <v>671399</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>282800</v>
+        <v>752000</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>584800</v>
+        <v>773501</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>195800</v>
+        <v>749000</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>335500</v>
+        <v>827300</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>792000</v>
+        <v>815200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>827999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>720600</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>809200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>158200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>976800</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1328399</v>
       </c>
     </row>
   </sheetData>
@@ -2477,7 +2592,7 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58C2D772-13F8-4778-9E3E-1BF0CA692876}">
-  <dimension ref="A1:B152"/>
+  <dimension ref="A1:B194"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -2499,761 +2614,971 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>5207200</v>
+        <v>805000</v>
       </c>
       <c r="B2">
-        <f>AVERAGE(A2:A152)</f>
-        <v>1672788.0794701986</v>
+        <f>AVERAGE(A2:A194)</f>
+        <v>1738588.0932642487</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1354800</v>
+        <v>2977000</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>12931000</v>
+        <v>3128900</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>780500</v>
+        <v>4633300</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4881500</v>
+        <v>5971800</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>3885200</v>
+        <v>4631599</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1269700</v>
+        <v>3175600</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>4129400</v>
+        <v>3094200</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1088200</v>
+        <v>2522601</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>757600</v>
+        <v>1798500</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>929700</v>
+        <v>3587300</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>876800</v>
+        <v>3474500</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>13582700</v>
+        <v>1011400</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>738400</v>
+        <v>838599</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2966600</v>
+        <v>2753501</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>3261600</v>
+        <v>456600</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>800900</v>
+        <v>638901</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2910300</v>
+        <v>2493300</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>1608100</v>
+        <v>983000</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>712600</v>
+        <v>1520599</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>613900</v>
+        <v>2834901</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>1407700</v>
+        <v>2609401</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>630000</v>
+        <v>1591899</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>845800</v>
+        <v>147300</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>772200</v>
+        <v>2747400</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>1150400</v>
+        <v>972200</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>559500</v>
+        <v>3159799</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>964800</v>
+        <v>1981600</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>475800</v>
+        <v>1970401</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>946100</v>
+        <v>2787800</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>862300</v>
+        <v>403300</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>637200</v>
+        <v>686900</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>551300</v>
+        <v>1211600</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>662700</v>
+        <v>2512201</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>541800</v>
+        <v>1005501</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>2576000</v>
+        <v>1116300</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>866900</v>
+        <v>2036000</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>2631200</v>
+        <v>1927100</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>472300</v>
+        <v>1657201</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>446500</v>
+        <v>1770600</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>2005700</v>
+        <v>2158800</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>2667200</v>
+        <v>1888499</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>384300</v>
+        <v>2119300</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>1021600</v>
+        <v>2062500</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>1040800</v>
+        <v>2224199</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>1130100</v>
+        <v>2928900</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>490500</v>
+        <v>414799</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>1071800</v>
+        <v>1168599</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>2506200</v>
+        <v>2133200</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>2466100</v>
+        <v>2575100</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>1840300</v>
+        <v>2179300</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>1370800</v>
+        <v>1430799</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>8634200</v>
+        <v>3442199</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>1138500</v>
+        <v>57200</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>5397400</v>
+        <v>2804300</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>459100</v>
+        <v>2838300</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>1270200</v>
+        <v>128500</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>2116000</v>
+        <v>1737600</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>1051600</v>
+        <v>2982500</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>537500</v>
+        <v>2227301</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>2990800</v>
+        <v>1697200</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>479900</v>
+        <v>2126700</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>855300</v>
+        <v>2390500</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>535900</v>
+        <v>2466300</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>610800</v>
+        <v>1004500</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>1017800</v>
+        <v>861900</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>569300</v>
+        <v>2314900</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>2010400</v>
+        <v>2123599</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>3026500</v>
+        <v>1331700</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>336700</v>
+        <v>467900</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>488400</v>
+        <v>683100</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>438100</v>
+        <v>2529601</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>2769100</v>
+        <v>3171501</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>4986800</v>
+        <v>3368300</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>1839600</v>
+        <v>3095399</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>406700</v>
+        <v>1101699</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>687700</v>
+        <v>553700</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>2525500</v>
+        <v>2018400</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>378300</v>
+        <v>2243700</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>544400</v>
+        <v>1791300</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>320500</v>
+        <v>1709301</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>1819200</v>
+        <v>765200</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>1055700</v>
+        <v>21028100</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>315500</v>
+        <v>2117999</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>1975500</v>
+        <v>1848100</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>365400</v>
+        <v>1749200</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>2725100</v>
+        <v>1383600</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>414500</v>
+        <v>1695201</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>2801700</v>
+        <v>508300</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>1199300</v>
+        <v>2100001</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>933000</v>
+        <v>1959000</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>461600</v>
+        <v>1391500</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>4510600</v>
+        <v>2025699</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>1524800</v>
+        <v>1265600</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>1992300</v>
+        <v>2272001</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>502000</v>
+        <v>322000</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>1559800</v>
+        <v>1638700</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>1886400</v>
+        <v>975600</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>411500</v>
+        <v>2026900</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>1955500</v>
+        <v>1012000</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>5836100</v>
+        <v>844100</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>658700</v>
+        <v>2131900</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>297100</v>
+        <v>1775200</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>2159800</v>
+        <v>1762500</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>1093200</v>
+        <v>362100</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>491000</v>
+        <v>1714200</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>376000</v>
+        <v>433600</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>3661900</v>
+        <v>891800</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>340200</v>
+        <v>490200</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>906600</v>
+        <v>424200</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>2119600</v>
+        <v>386300</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>981600</v>
+        <v>1751599</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>4778800</v>
+        <v>338899</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>1888500</v>
+        <v>2114299</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>1682800</v>
+        <v>1798499</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>884900</v>
+        <v>1597000</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>762100</v>
+        <v>2013200</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>1792500</v>
+        <v>2056300</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>5369600</v>
+        <v>1884800</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>1682400</v>
+        <v>1695900</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122">
-        <v>900100</v>
+        <v>1516801</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>379100</v>
+        <v>1548201</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>1849500</v>
+        <v>1862600</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>894100</v>
+        <v>1447300</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>2055100</v>
+        <v>301000</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>349500</v>
+        <v>2249700</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>512500</v>
+        <v>2084000</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>5298700</v>
+        <v>179600</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>4821900</v>
+        <v>1552401</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>843800</v>
+        <v>1580900</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>4829000</v>
+        <v>1795901</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>328800</v>
+        <v>2077399</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>300800</v>
+        <v>1470501</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>359100</v>
+        <v>1002800</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>493400</v>
+        <v>1392499</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>323800</v>
+        <v>2794700</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138">
-        <v>339400</v>
+        <v>1874900</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>808500</v>
+        <v>1552901</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>305900</v>
+        <v>1817700</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>344700</v>
+        <v>1534400</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>346900</v>
+        <v>1670401</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143">
-        <v>2237500</v>
+        <v>1729900</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144">
-        <v>1561300</v>
+        <v>1711900</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>667600</v>
+        <v>2433700</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146">
-        <v>1127800</v>
+        <v>1946100</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147">
-        <v>1857200</v>
+        <v>1873300</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148">
-        <v>319200</v>
+        <v>366000</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149">
-        <v>581700</v>
+        <v>2531500</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>412800</v>
+        <v>1997700</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151">
-        <v>567200</v>
+        <v>620800</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152">
-        <v>695700</v>
+        <v>319100</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>589501</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>1536599</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>2003201</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>651801</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>2121800</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>1773600</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>970300</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>1956900</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>1467200</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>1884100</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>354900</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>299600</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>1271499</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>972600</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>718300</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>814600</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>721700</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>1404501</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>2016600</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>877100</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>1293800</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>1174900</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>1700600</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>1990200</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>381700</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>597900</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>1654400</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>289200</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>2264400</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>1627900</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>2178901</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>379099</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>421000</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>140000</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>1754099</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>1424200</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>1928900</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>280099</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>683900</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>299101</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>991000</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>119200</v>
       </c>
     </row>
   </sheetData>
@@ -3263,10 +3588,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D5D9261-0F86-4536-90B1-950DFA9F85C0}">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3284,202 +3609,8 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1888900</v>
-      </c>
-      <c r="B2">
-        <f>AVERAGE(A2:A40)</f>
-        <v>606092.30769230775</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>202400</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>796400</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>72800</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>89400</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>7300</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>6500</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>13600</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10300</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>31700</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>17800</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>34200</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>38100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>9200</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>47400</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>59200</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>16900</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19488400</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>21100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>27500</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>22200</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>41700</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>42400</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>29100</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>31200</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>10400</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>52700</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>46500</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>25500</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>38000</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>50000</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>45500</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>45900</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>10400</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>26500</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>88700</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>134800</v>
+      <c r="B2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -3492,7 +3623,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3511,106 +3642,106 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1040464886526000</v>
+        <v>1121017383806100</v>
       </c>
       <c r="B2">
         <f>AVERAGE(A2:A21)</f>
-        <v>1040532417227865</v>
+        <v>1121109266559524</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1040479893483100</v>
+        <v>1121247553998600</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1040509910035000</v>
+        <v>1121034398015100</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1040479893483100</v>
+        <v>1121066424183000</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1040464886526000</v>
+        <v>1121034398015100</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1040544934556100</v>
+        <v>1121017383806100</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1040559947844300</v>
+        <v>1121103449237800</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1040456825951300</v>
+        <v>1120999357969200</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1040486842998100</v>
+        <v>1121114328683600</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1040681943827100</v>
+        <v>1121034342251200</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>1040443823063600</v>
+        <v>1121090386519600</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>1040593843662900</v>
+        <v>1121078382033890</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>1040533837387000</v>
+        <v>1121010318990500</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>1040558837693100</v>
+        <v>1121041352256000</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>1040513832800700</v>
+        <v>1121194466649300</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>1040593843662900</v>
+        <v>1121078382033890</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>1040573838692400</v>
+        <v>1121260512576800</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>1040553839861500</v>
+        <v>1121236490451100</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>1040563839962600</v>
+        <v>1121248501910500</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>1040588842540500</v>
+        <v>1121277517803100</v>
       </c>
     </row>
   </sheetData>
@@ -3623,7 +3754,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3642,11 +3773,11 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>600</v>
+        <v>1901</v>
       </c>
       <c r="B2">
         <f>AVERAGE(A2:A2)</f>
-        <v>600</v>
+        <v>1901</v>
       </c>
     </row>
   </sheetData>
@@ -3678,11 +3809,11 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>95900</v>
+        <v>57300</v>
       </c>
       <c r="B2">
         <f>AVERAGE(A2)</f>
-        <v>95900</v>
+        <v>57300</v>
       </c>
     </row>
   </sheetData>
@@ -3746,16 +3877,16 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1583000</v>
+        <v>4115100</v>
       </c>
       <c r="B2">
         <f>AVERAGE(A2:A3)</f>
-        <v>883300</v>
+        <v>2360200</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>183600</v>
+        <v>605300</v>
       </c>
     </row>
   </sheetData>
@@ -3787,11 +3918,11 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>779200</v>
+        <v>673700</v>
       </c>
       <c r="B2">
         <f>AVERAGE(A2)</f>
-        <v>779200</v>
+        <v>673700</v>
       </c>
     </row>
   </sheetData>
@@ -3855,106 +3986,106 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>7285763400</v>
+        <v>3384603600</v>
       </c>
       <c r="B2">
         <f>AVERAGE(A2:A21)</f>
-        <v>1741127575</v>
+        <v>2352538545.0999999</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>976355200</v>
+        <v>3985233600</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>966348300</v>
+        <v>4975631900</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>997060300</v>
+        <v>961795599</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1987172900</v>
+        <v>1955700200</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>985158500</v>
+        <v>1981827501</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>966620200</v>
+        <v>2974857901</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>945934000</v>
+        <v>946068901</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>960507600</v>
+        <v>1944310300</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1953697300</v>
+        <v>2938963501</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>960796600</v>
+        <v>918795500</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>951270600</v>
+        <v>1913819000</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>1938040600</v>
+        <v>899754500</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>937285000</v>
+        <v>1897643799</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>1925649900</v>
+        <v>887170200</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>423934800</v>
+        <v>3000822600</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>919393000</v>
+        <v>3880827800</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>1919580200</v>
+        <v>2872251300</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>2912235500</v>
+        <v>1867743300</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>3909747600</v>
+        <v>2862949900</v>
       </c>
     </row>
   </sheetData>

</xml_diff>